<commit_message>
Commit con visualizacion de errores relativos
</commit_message>
<xml_diff>
--- a/casos_de_estudio/caso_1/errores.xlsx
+++ b/casos_de_estudio/caso_1/errores.xlsx
@@ -452,16 +452,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B2" t="n">
-        <v>2380000</v>
+        <v>2233000</v>
       </c>
       <c r="C2" t="n">
-        <v>4424403.5</v>
+        <v>4321220</v>
       </c>
       <c r="D2" t="n">
-        <v>85.89930672268908</v>
+        <v>93.51634572324228</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>1750000</v>
       </c>
       <c r="C3" t="n">
-        <v>3191166</v>
+        <v>3380407.25</v>
       </c>
       <c r="D3" t="n">
-        <v>82.35234285714286</v>
+        <v>93.16612857142857</v>
       </c>
     </row>
     <row r="4">
@@ -486,52 +486,52 @@
         <v>1750000</v>
       </c>
       <c r="C4" t="n">
-        <v>3128690.25</v>
+        <v>3272603</v>
       </c>
       <c r="D4" t="n">
-        <v>78.78230000000001</v>
+        <v>87.00588571428571</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B5" t="n">
-        <v>2233000</v>
+        <v>2380000</v>
       </c>
       <c r="C5" t="n">
-        <v>3838530.75</v>
+        <v>4371614.5</v>
       </c>
       <c r="D5" t="n">
-        <v>71.90016793551275</v>
+        <v>83.68128151260504</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>1750000</v>
+        <v>3500000</v>
       </c>
       <c r="C6" t="n">
-        <v>2996142.75</v>
+        <v>5932616</v>
       </c>
       <c r="D6" t="n">
-        <v>71.20815714285715</v>
+        <v>69.5033142857143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="B7" t="n">
-        <v>3500000</v>
+        <v>1750000</v>
       </c>
       <c r="C7" t="n">
-        <v>5517755.5</v>
+        <v>2822316</v>
       </c>
       <c r="D7" t="n">
-        <v>57.65015714285714</v>
+        <v>61.2752</v>
       </c>
     </row>
     <row r="8">
@@ -542,38 +542,38 @@
         <v>2275000</v>
       </c>
       <c r="C8" t="n">
-        <v>3534750.5</v>
+        <v>3535271.25</v>
       </c>
       <c r="D8" t="n">
-        <v>55.37364835164836</v>
+        <v>55.39653846153846</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="B9" t="n">
-        <v>1890000</v>
+        <v>8400000</v>
       </c>
       <c r="C9" t="n">
-        <v>2912904.75</v>
+        <v>4119406.75</v>
       </c>
       <c r="D9" t="n">
-        <v>54.12194444444446</v>
+        <v>50.95944345238095</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B10" t="n">
-        <v>8400000</v>
+        <v>2520000</v>
       </c>
       <c r="C10" t="n">
-        <v>4136360.5</v>
+        <v>3699640.75</v>
       </c>
       <c r="D10" t="n">
-        <v>50.7576130952381</v>
+        <v>46.81114087301587</v>
       </c>
     </row>
     <row r="11">
@@ -584,94 +584,94 @@
         <v>4025000</v>
       </c>
       <c r="C11" t="n">
-        <v>5937514</v>
+        <v>5738945.5</v>
       </c>
       <c r="D11" t="n">
-        <v>47.51587577639751</v>
+        <v>42.58249689440994</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B12" t="n">
-        <v>3570000</v>
+        <v>4340000</v>
       </c>
       <c r="C12" t="n">
-        <v>5241221.5</v>
+        <v>6158072.5</v>
       </c>
       <c r="D12" t="n">
-        <v>46.81292717086833</v>
+        <v>41.89107142857143</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B13" t="n">
-        <v>4340000</v>
+        <v>3570000</v>
       </c>
       <c r="C13" t="n">
-        <v>6370170</v>
+        <v>5003962.5</v>
       </c>
       <c r="D13" t="n">
-        <v>46.77811059907835</v>
+        <v>40.16701680672267</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="B14" t="n">
-        <v>2450000</v>
+        <v>1890000</v>
       </c>
       <c r="C14" t="n">
-        <v>3580393.5</v>
+        <v>2630729.75</v>
       </c>
       <c r="D14" t="n">
-        <v>46.13851020408163</v>
+        <v>39.19205026455028</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B15" t="n">
-        <v>3080000</v>
+        <v>2450000</v>
       </c>
       <c r="C15" t="n">
-        <v>4476866.5</v>
+        <v>3392808.75</v>
       </c>
       <c r="D15" t="n">
-        <v>45.35280844155844</v>
+        <v>38.48198979591837</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="B16" t="n">
-        <v>2520000</v>
+        <v>4200000</v>
       </c>
       <c r="C16" t="n">
-        <v>3662826.75</v>
+        <v>5768288</v>
       </c>
       <c r="D16" t="n">
-        <v>45.35026785714285</v>
+        <v>37.34019047619048</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>4200000</v>
+        <v>3010000</v>
       </c>
       <c r="C17" t="n">
-        <v>5899988</v>
+        <v>4128174.5</v>
       </c>
       <c r="D17" t="n">
-        <v>40.47590476190476</v>
+        <v>37.14865448504983</v>
       </c>
     </row>
     <row r="18">
@@ -682,584 +682,584 @@
         <v>2450000</v>
       </c>
       <c r="C18" t="n">
-        <v>3410046</v>
+        <v>3340312.5</v>
       </c>
       <c r="D18" t="n">
-        <v>39.18555102040816</v>
+        <v>36.33928571428572</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B19" t="n">
-        <v>3850000</v>
+        <v>5110000</v>
       </c>
       <c r="C19" t="n">
-        <v>5226674</v>
+        <v>3332437.25</v>
       </c>
       <c r="D19" t="n">
-        <v>35.75776623376623</v>
+        <v>34.78596379647749</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="B20" t="n">
-        <v>2135000</v>
+        <v>3080000</v>
       </c>
       <c r="C20" t="n">
-        <v>2890783.25</v>
+        <v>4132898</v>
       </c>
       <c r="D20" t="n">
-        <v>35.39968384074941</v>
+        <v>34.185</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B21" t="n">
-        <v>3430000</v>
+        <v>3850000</v>
       </c>
       <c r="C21" t="n">
-        <v>4583918</v>
+        <v>5140917.5</v>
       </c>
       <c r="D21" t="n">
-        <v>33.64192419825073</v>
+        <v>33.53032467532467</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B22" t="n">
-        <v>4543000</v>
+        <v>2135000</v>
       </c>
       <c r="C22" t="n">
-        <v>6056867.5</v>
+        <v>2782056</v>
       </c>
       <c r="D22" t="n">
-        <v>33.32307946290997</v>
+        <v>30.30707259953162</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B23" t="n">
-        <v>3010000</v>
+        <v>3500000</v>
       </c>
       <c r="C23" t="n">
-        <v>3995510.75</v>
+        <v>4558037</v>
       </c>
       <c r="D23" t="n">
-        <v>32.74122093023256</v>
+        <v>30.22962857142857</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B24" t="n">
-        <v>8680000</v>
+        <v>2870000</v>
       </c>
       <c r="C24" t="n">
-        <v>5955111.5</v>
+        <v>3716983.5</v>
       </c>
       <c r="D24" t="n">
-        <v>31.39272465437788</v>
+        <v>29.51162020905923</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B25" t="n">
-        <v>3080000</v>
+        <v>3290000</v>
       </c>
       <c r="C25" t="n">
-        <v>4033428.75</v>
+        <v>4245402</v>
       </c>
       <c r="D25" t="n">
-        <v>30.95547889610389</v>
+        <v>29.03957446808511</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="B26" t="n">
-        <v>3640000</v>
+        <v>8680000</v>
       </c>
       <c r="C26" t="n">
-        <v>4756747</v>
+        <v>6177615</v>
       </c>
       <c r="D26" t="n">
-        <v>30.67986263736262</v>
+        <v>28.82932027649769</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B27" t="n">
-        <v>5110000</v>
+        <v>3430000</v>
       </c>
       <c r="C27" t="n">
-        <v>3546918.75</v>
+        <v>4388945.5</v>
       </c>
       <c r="D27" t="n">
-        <v>30.58867416829746</v>
+        <v>27.95759475218659</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B28" t="n">
-        <v>2485000</v>
+        <v>4543000</v>
       </c>
       <c r="C28" t="n">
-        <v>3198830.25</v>
+        <v>5811781.5</v>
       </c>
       <c r="D28" t="n">
-        <v>28.72556338028169</v>
+        <v>27.92827426810478</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B29" t="n">
-        <v>4375000</v>
+        <v>3080000</v>
       </c>
       <c r="C29" t="n">
-        <v>3136273.5</v>
+        <v>3918247.75</v>
       </c>
       <c r="D29" t="n">
-        <v>28.31374857142857</v>
+        <v>27.21583603896104</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B30" t="n">
-        <v>2870000</v>
+        <v>5600000</v>
       </c>
       <c r="C30" t="n">
-        <v>3658486.5</v>
+        <v>4100026.25</v>
       </c>
       <c r="D30" t="n">
-        <v>27.47339721254355</v>
+        <v>26.78524553571429</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B31" t="n">
-        <v>4970000</v>
+        <v>2870000</v>
       </c>
       <c r="C31" t="n">
-        <v>6312960</v>
+        <v>3598649.5</v>
       </c>
       <c r="D31" t="n">
-        <v>27.02132796780684</v>
+        <v>25.38848432055749</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="B32" t="n">
-        <v>4060000</v>
+        <v>4375000</v>
       </c>
       <c r="C32" t="n">
-        <v>5155119</v>
+        <v>3283094.5</v>
       </c>
       <c r="D32" t="n">
-        <v>26.97337438423645</v>
+        <v>24.95784</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="B33" t="n">
-        <v>3290000</v>
+        <v>3990000</v>
       </c>
       <c r="C33" t="n">
-        <v>4146467.25</v>
+        <v>4984787</v>
       </c>
       <c r="D33" t="n">
-        <v>26.03243920972644</v>
+        <v>24.93200501253133</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>3990000</v>
+        <v>3640000</v>
       </c>
       <c r="C34" t="n">
-        <v>4973159.5</v>
+        <v>4508519.5</v>
       </c>
       <c r="D34" t="n">
-        <v>24.64058897243108</v>
+        <v>23.86042582417581</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="B35" t="n">
-        <v>3920000</v>
+        <v>5033000</v>
       </c>
       <c r="C35" t="n">
-        <v>4852118</v>
+        <v>3866840.75</v>
       </c>
       <c r="D35" t="n">
-        <v>23.77852040816326</v>
+        <v>23.17026127558116</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="B36" t="n">
-        <v>5600000</v>
+        <v>2485000</v>
       </c>
       <c r="C36" t="n">
-        <v>4270943</v>
+        <v>3055258.25</v>
       </c>
       <c r="D36" t="n">
-        <v>23.73316071428571</v>
+        <v>22.94801810865191</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B37" t="n">
-        <v>3500000</v>
+        <v>8294999.999999999</v>
       </c>
       <c r="C37" t="n">
-        <v>4257108.5</v>
+        <v>6462561.5</v>
       </c>
       <c r="D37" t="n">
-        <v>21.63167142857143</v>
+        <v>22.09088004822181</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="B38" t="n">
-        <v>2408000</v>
+        <v>3703000</v>
       </c>
       <c r="C38" t="n">
-        <v>2928118.25</v>
+        <v>4501734.5</v>
       </c>
       <c r="D38" t="n">
-        <v>21.59959509966777</v>
+        <v>21.56992978665948</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="B39" t="n">
-        <v>5495000</v>
+        <v>3290000</v>
       </c>
       <c r="C39" t="n">
-        <v>4350131</v>
+        <v>3967805.25</v>
       </c>
       <c r="D39" t="n">
-        <v>20.8347406733394</v>
+        <v>20.60198328267477</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B40" t="n">
-        <v>3290000</v>
+        <v>3640000</v>
       </c>
       <c r="C40" t="n">
-        <v>3960702.25</v>
+        <v>4362461.5</v>
       </c>
       <c r="D40" t="n">
-        <v>20.38608662613982</v>
+        <v>19.84784340659339</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="B41" t="n">
-        <v>8294999.999999999</v>
+        <v>3710000</v>
       </c>
       <c r="C41" t="n">
-        <v>6640106</v>
+        <v>2978359.75</v>
       </c>
       <c r="D41" t="n">
-        <v>19.95050030138637</v>
+        <v>19.7207614555256</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>5810000</v>
+        <v>5530000</v>
       </c>
       <c r="C42" t="n">
-        <v>4693662</v>
+        <v>4461440.5</v>
       </c>
       <c r="D42" t="n">
-        <v>19.21407917383821</v>
+        <v>19.32295660036166</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="B43" t="n">
-        <v>4690000</v>
+        <v>5950000</v>
       </c>
       <c r="C43" t="n">
-        <v>3793510.5</v>
+        <v>4830545</v>
       </c>
       <c r="D43" t="n">
-        <v>19.11491471215352</v>
+        <v>18.81436974789916</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B44" t="n">
-        <v>3465000</v>
+        <v>5565000</v>
       </c>
       <c r="C44" t="n">
-        <v>4122910.5</v>
+        <v>6569257.5</v>
       </c>
       <c r="D44" t="n">
-        <v>18.98731601731602</v>
+        <v>18.04595687331537</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B45" t="n">
-        <v>5390000</v>
+        <v>4690000</v>
       </c>
       <c r="C45" t="n">
-        <v>6393535</v>
+        <v>3860289.5</v>
       </c>
       <c r="D45" t="n">
-        <v>18.61846011131725</v>
+        <v>17.69105543710021</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="B46" t="n">
-        <v>5250000</v>
+        <v>5215000</v>
       </c>
       <c r="C46" t="n">
-        <v>6225744.5</v>
+        <v>4305643.5</v>
       </c>
       <c r="D46" t="n">
-        <v>18.58560952380952</v>
+        <v>17.43732502396932</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B47" t="n">
-        <v>2590000</v>
+        <v>5495000</v>
       </c>
       <c r="C47" t="n">
-        <v>3070216.25</v>
+        <v>4548168.5</v>
       </c>
       <c r="D47" t="n">
-        <v>18.54116795366795</v>
+        <v>17.23078252957234</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B48" t="n">
-        <v>4473000</v>
+        <v>7245000</v>
       </c>
       <c r="C48" t="n">
-        <v>5281724</v>
+        <v>8487414</v>
       </c>
       <c r="D48" t="n">
-        <v>18.08012519561816</v>
+        <v>17.14857142857143</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B49" t="n">
-        <v>2870000</v>
+        <v>2408000</v>
       </c>
       <c r="C49" t="n">
-        <v>3388169.75</v>
+        <v>2816920.25</v>
       </c>
       <c r="D49" t="n">
-        <v>18.05469512195122</v>
+        <v>16.98173795681063</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B50" t="n">
-        <v>6930000</v>
+        <v>6300000</v>
       </c>
       <c r="C50" t="n">
-        <v>5739791</v>
+        <v>5252373</v>
       </c>
       <c r="D50" t="n">
-        <v>17.17473304473305</v>
+        <v>16.629</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="B51" t="n">
-        <v>7245000</v>
+        <v>6650000</v>
       </c>
       <c r="C51" t="n">
-        <v>8456038</v>
+        <v>5554134</v>
       </c>
       <c r="D51" t="n">
-        <v>16.71550034506556</v>
+        <v>16.47918796992481</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B52" t="n">
-        <v>6300000</v>
+        <v>4060000</v>
       </c>
       <c r="C52" t="n">
-        <v>5280426</v>
+        <v>3407564.5</v>
       </c>
       <c r="D52" t="n">
-        <v>16.18371428571428</v>
+        <v>16.06983990147783</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="B53" t="n">
-        <v>5033000</v>
+        <v>5390000</v>
       </c>
       <c r="C53" t="n">
-        <v>4223660.5</v>
+        <v>6251707</v>
       </c>
       <c r="D53" t="n">
-        <v>16.08065765944765</v>
+        <v>15.98714285714286</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B54" t="n">
-        <v>4200000</v>
+        <v>6419000</v>
       </c>
       <c r="C54" t="n">
-        <v>3526730.75</v>
+        <v>5408772.5</v>
       </c>
       <c r="D54" t="n">
-        <v>16.03022023809524</v>
+        <v>15.73808225580308</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="B55" t="n">
-        <v>3885000</v>
+        <v>3430000</v>
       </c>
       <c r="C55" t="n">
-        <v>4495333</v>
+        <v>2903050.5</v>
       </c>
       <c r="D55" t="n">
-        <v>15.70998712998713</v>
+        <v>15.36295918367347</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B56" t="n">
-        <v>3640000</v>
+        <v>3885000</v>
       </c>
       <c r="C56" t="n">
-        <v>4207608</v>
+        <v>4466045</v>
       </c>
       <c r="D56" t="n">
-        <v>15.59362637362636</v>
+        <v>14.95611325611326</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B57" t="n">
-        <v>5810000</v>
+        <v>6930000</v>
       </c>
       <c r="C57" t="n">
-        <v>4910560</v>
+        <v>5912520.5</v>
       </c>
       <c r="D57" t="n">
-        <v>15.48089500860585</v>
+        <v>14.68224386724387</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B58" t="n">
-        <v>5740000</v>
+        <v>3465000</v>
       </c>
       <c r="C58" t="n">
-        <v>4856403.5</v>
+        <v>3964181.25</v>
       </c>
       <c r="D58" t="n">
-        <v>15.39366724738676</v>
+        <v>14.40638528138528</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="B59" t="n">
-        <v>5950000</v>
+        <v>2835000</v>
       </c>
       <c r="C59" t="n">
-        <v>5035798.5</v>
+        <v>3240659</v>
       </c>
       <c r="D59" t="n">
-        <v>15.36473109243698</v>
+        <v>14.3089594356261</v>
       </c>
     </row>
     <row r="60">
@@ -1270,780 +1270,780 @@
         <v>4907000</v>
       </c>
       <c r="C60" t="n">
-        <v>4163627.5</v>
+        <v>4205315.5</v>
       </c>
       <c r="D60" t="n">
-        <v>15.14922559608722</v>
+        <v>14.29966374566945</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>6650000</v>
+        <v>3087000</v>
       </c>
       <c r="C61" t="n">
-        <v>5645206</v>
+        <v>3522897.75</v>
       </c>
       <c r="D61" t="n">
-        <v>15.10968421052632</v>
+        <v>14.12043245869777</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B62" t="n">
-        <v>2660000</v>
+        <v>5250000</v>
       </c>
       <c r="C62" t="n">
-        <v>3061633.25</v>
+        <v>5983282</v>
       </c>
       <c r="D62" t="n">
-        <v>15.09899436090226</v>
+        <v>13.96727619047619</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="B63" t="n">
-        <v>3675000</v>
+        <v>3920000</v>
       </c>
       <c r="C63" t="n">
-        <v>4227608.5</v>
+        <v>4450266</v>
       </c>
       <c r="D63" t="n">
-        <v>15.03696598639457</v>
+        <v>13.52719387755102</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>6419000</v>
+        <v>5810000</v>
       </c>
       <c r="C64" t="n">
-        <v>5461532</v>
+        <v>5033414</v>
       </c>
       <c r="D64" t="n">
-        <v>14.91615516435582</v>
+        <v>13.36636833046471</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B65" t="n">
-        <v>4403000</v>
+        <v>4200000</v>
       </c>
       <c r="C65" t="n">
-        <v>3776033.5</v>
+        <v>3638951.25</v>
       </c>
       <c r="D65" t="n">
-        <v>14.23952986600046</v>
+        <v>13.35830357142857</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B66" t="n">
-        <v>5460000</v>
+        <v>2590000</v>
       </c>
       <c r="C66" t="n">
-        <v>6218641</v>
+        <v>2933935.25</v>
       </c>
       <c r="D66" t="n">
-        <v>13.89452380952381</v>
+        <v>13.27935328185328</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="B67" t="n">
-        <v>3675000</v>
+        <v>4060000</v>
       </c>
       <c r="C67" t="n">
-        <v>3169733.25</v>
+        <v>4577985.5</v>
       </c>
       <c r="D67" t="n">
-        <v>13.74875510204081</v>
+        <v>12.75826354679803</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B68" t="n">
-        <v>5950000</v>
+        <v>2940000</v>
       </c>
       <c r="C68" t="n">
-        <v>5132399</v>
+        <v>3297328.75</v>
       </c>
       <c r="D68" t="n">
-        <v>13.74119327731092</v>
+        <v>12.15403911564626</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>84</v>
+        <v>16</v>
       </c>
       <c r="B69" t="n">
-        <v>5565000</v>
+        <v>5460000</v>
       </c>
       <c r="C69" t="n">
-        <v>6269683.5</v>
+        <v>6122246.5</v>
       </c>
       <c r="D69" t="n">
-        <v>12.66277628032345</v>
+        <v>12.12905677655678</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B70" t="n">
-        <v>4095000</v>
+        <v>5950000</v>
       </c>
       <c r="C70" t="n">
-        <v>4599195</v>
+        <v>5228970</v>
       </c>
       <c r="D70" t="n">
-        <v>12.31245421245421</v>
+        <v>12.1181512605042</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B71" t="n">
-        <v>3087000</v>
+        <v>8400000</v>
       </c>
       <c r="C71" t="n">
-        <v>3465336.75</v>
+        <v>7413476</v>
       </c>
       <c r="D71" t="n">
-        <v>12.25580660835763</v>
+        <v>11.74433333333333</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B72" t="n">
-        <v>6090000</v>
+        <v>4550000</v>
       </c>
       <c r="C72" t="n">
-        <v>5352505.5</v>
+        <v>5068953</v>
       </c>
       <c r="D72" t="n">
-        <v>12.10992610837438</v>
+        <v>11.40556043956044</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="B73" t="n">
-        <v>3710000</v>
+        <v>3360000</v>
       </c>
       <c r="C73" t="n">
-        <v>3265717.75</v>
+        <v>2979431</v>
       </c>
       <c r="D73" t="n">
-        <v>11.97526280323449</v>
+        <v>11.32645833333333</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B74" t="n">
-        <v>2940000</v>
+        <v>3780000</v>
       </c>
       <c r="C74" t="n">
-        <v>3281655.25</v>
+        <v>4203505.5</v>
       </c>
       <c r="D74" t="n">
-        <v>11.6209268707483</v>
+        <v>11.20384920634922</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B75" t="n">
-        <v>3703000</v>
+        <v>3675000</v>
       </c>
       <c r="C75" t="n">
-        <v>4131040.75</v>
+        <v>4085956.25</v>
       </c>
       <c r="D75" t="n">
-        <v>11.55929651633812</v>
+        <v>11.18248299319729</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="B76" t="n">
-        <v>4060000</v>
+        <v>4970000</v>
       </c>
       <c r="C76" t="n">
-        <v>3612686.5</v>
+        <v>5518557.5</v>
       </c>
       <c r="D76" t="n">
-        <v>11.01757389162562</v>
+        <v>11.03737424547284</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B77" t="n">
-        <v>4480000</v>
+        <v>3675000</v>
       </c>
       <c r="C77" t="n">
-        <v>4012459.25</v>
+        <v>3271173</v>
       </c>
       <c r="D77" t="n">
-        <v>10.43617745535714</v>
+        <v>10.98848979591836</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B78" t="n">
-        <v>5530000</v>
+        <v>7419999.999999999</v>
       </c>
       <c r="C78" t="n">
-        <v>4974849.5</v>
+        <v>6640457.5</v>
       </c>
       <c r="D78" t="n">
-        <v>10.03888788426763</v>
+        <v>10.50596361185983</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B79" t="n">
-        <v>2835000</v>
+        <v>6090000</v>
       </c>
       <c r="C79" t="n">
-        <v>3091513</v>
+        <v>5455917.5</v>
       </c>
       <c r="D79" t="n">
-        <v>9.048077601410935</v>
+        <v>10.41186371100164</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B80" t="n">
-        <v>6020000</v>
+        <v>3115000</v>
       </c>
       <c r="C80" t="n">
-        <v>5482883.5</v>
+        <v>2804314.5</v>
       </c>
       <c r="D80" t="n">
-        <v>8.922200996677741</v>
+        <v>9.973852327447833</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B81" t="n">
-        <v>4270000</v>
+        <v>4403000</v>
       </c>
       <c r="C81" t="n">
-        <v>4638077</v>
+        <v>3966234.75</v>
       </c>
       <c r="D81" t="n">
-        <v>8.620070257611241</v>
+        <v>9.919719509425391</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B82" t="n">
-        <v>4550000</v>
+        <v>5950000</v>
       </c>
       <c r="C82" t="n">
-        <v>4941898</v>
+        <v>5411614</v>
       </c>
       <c r="D82" t="n">
-        <v>8.613142857142856</v>
+        <v>9.048504201680672</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B83" t="n">
-        <v>4550000</v>
+        <v>4480000</v>
       </c>
       <c r="C83" t="n">
-        <v>4923227.5</v>
+        <v>4078036.75</v>
       </c>
       <c r="D83" t="n">
-        <v>8.202802197802198</v>
+        <v>8.972393973214286</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B84" t="n">
-        <v>3430000</v>
+        <v>4550000</v>
       </c>
       <c r="C84" t="n">
-        <v>3148804.5</v>
+        <v>4943000</v>
       </c>
       <c r="D84" t="n">
-        <v>8.198119533527697</v>
+        <v>8.637362637362637</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B85" t="n">
-        <v>5250000</v>
+        <v>3535000</v>
       </c>
       <c r="C85" t="n">
-        <v>4826379</v>
+        <v>3237278.25</v>
       </c>
       <c r="D85" t="n">
-        <v>8.068971428571428</v>
+        <v>8.42211456859973</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="B86" t="n">
-        <v>5215000</v>
+        <v>3010000</v>
       </c>
       <c r="C86" t="n">
-        <v>4810805.5</v>
+        <v>3250350.25</v>
       </c>
       <c r="D86" t="n">
-        <v>7.750613614573346</v>
+        <v>7.985058139534884</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="B87" t="n">
-        <v>5880000</v>
+        <v>5950000</v>
       </c>
       <c r="C87" t="n">
-        <v>6334210.5</v>
+        <v>5478679</v>
       </c>
       <c r="D87" t="n">
-        <v>7.724668367346939</v>
+        <v>7.921361344537815</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B88" t="n">
-        <v>3780000</v>
+        <v>6510000</v>
       </c>
       <c r="C88" t="n">
-        <v>4066966.5</v>
+        <v>7001141.5</v>
       </c>
       <c r="D88" t="n">
-        <v>7.591706349206362</v>
+        <v>7.544416282642088</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="B89" t="n">
-        <v>4690000</v>
+        <v>6293000</v>
       </c>
       <c r="C89" t="n">
-        <v>4339585</v>
+        <v>6760827</v>
       </c>
       <c r="D89" t="n">
-        <v>7.471535181236674</v>
+        <v>7.434085491816305</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="B90" t="n">
-        <v>3360000</v>
+        <v>3605000</v>
       </c>
       <c r="C90" t="n">
-        <v>3109125.25</v>
+        <v>3864727.25</v>
       </c>
       <c r="D90" t="n">
-        <v>7.466510416666666</v>
+        <v>7.204639389736463</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="B91" t="n">
-        <v>2940000</v>
+        <v>4473000</v>
       </c>
       <c r="C91" t="n">
-        <v>3159124</v>
+        <v>4784397.5</v>
       </c>
       <c r="D91" t="n">
-        <v>7.453197278911565</v>
+        <v>6.961714732841494</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="B92" t="n">
-        <v>3535000</v>
+        <v>4900000</v>
       </c>
       <c r="C92" t="n">
-        <v>3277594</v>
+        <v>4559873.5</v>
       </c>
       <c r="D92" t="n">
-        <v>7.281640735502134</v>
+        <v>6.941357142857142</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="B93" t="n">
-        <v>7840000</v>
+        <v>4095000</v>
       </c>
       <c r="C93" t="n">
-        <v>7286088</v>
+        <v>4376780.5</v>
       </c>
       <c r="D93" t="n">
-        <v>7.065204081632653</v>
+        <v>6.881086691086691</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B94" t="n">
-        <v>6930000</v>
+        <v>6020000</v>
       </c>
       <c r="C94" t="n">
-        <v>6445524.5</v>
+        <v>5608299.5</v>
       </c>
       <c r="D94" t="n">
-        <v>6.990988455988456</v>
+        <v>6.838878737541529</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="B95" t="n">
-        <v>5040000</v>
+        <v>5250000</v>
       </c>
       <c r="C95" t="n">
-        <v>4707199</v>
+        <v>4904728.5</v>
       </c>
       <c r="D95" t="n">
-        <v>6.603194444444445</v>
+        <v>6.576600000000001</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="B96" t="n">
-        <v>4480000</v>
+        <v>4690000</v>
       </c>
       <c r="C96" t="n">
-        <v>4204255</v>
+        <v>4386747</v>
       </c>
       <c r="D96" t="n">
-        <v>6.155022321428572</v>
+        <v>6.46594882729211</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B97" t="n">
-        <v>4095000</v>
+        <v>5880000</v>
       </c>
       <c r="C97" t="n">
-        <v>4321394</v>
+        <v>6252206.5</v>
       </c>
       <c r="D97" t="n">
-        <v>5.528547008547009</v>
+        <v>6.330042517006802</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="B98" t="n">
-        <v>3353000</v>
+        <v>3500000</v>
       </c>
       <c r="C98" t="n">
-        <v>3171642.5</v>
+        <v>3721372.75</v>
       </c>
       <c r="D98" t="n">
-        <v>5.408813003280645</v>
+        <v>6.324935714285715</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B99" t="n">
-        <v>3605000</v>
+        <v>5810000</v>
       </c>
       <c r="C99" t="n">
-        <v>3797978.75</v>
+        <v>5456876.5</v>
       </c>
       <c r="D99" t="n">
-        <v>5.353085991678211</v>
+        <v>6.077857142857143</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B100" t="n">
-        <v>4200000</v>
+        <v>7840000</v>
       </c>
       <c r="C100" t="n">
-        <v>3978156.75</v>
+        <v>7374629.5</v>
       </c>
       <c r="D100" t="n">
-        <v>5.281982142857143</v>
+        <v>5.935848214285714</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>12</v>
+        <v>97</v>
       </c>
       <c r="B101" t="n">
-        <v>6300000</v>
+        <v>5740000</v>
       </c>
       <c r="C101" t="n">
-        <v>6614908.5</v>
+        <v>5414963</v>
       </c>
       <c r="D101" t="n">
-        <v>4.998547619047619</v>
+        <v>5.662665505226481</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B102" t="n">
-        <v>3703000</v>
+        <v>4270000</v>
       </c>
       <c r="C102" t="n">
-        <v>3885462.25</v>
+        <v>4509208.5</v>
       </c>
       <c r="D102" t="n">
-        <v>4.927416959222265</v>
+        <v>5.602072599531615</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="B103" t="n">
-        <v>8400000</v>
+        <v>4480000</v>
       </c>
       <c r="C103" t="n">
-        <v>7988711</v>
+        <v>4232415.5</v>
       </c>
       <c r="D103" t="n">
-        <v>4.896297619047619</v>
+        <v>5.526439732142857</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B104" t="n">
-        <v>4340000</v>
+        <v>8080940.000000001</v>
       </c>
       <c r="C104" t="n">
-        <v>4550580.5</v>
+        <v>7636855.5</v>
       </c>
       <c r="D104" t="n">
-        <v>4.852085253456221</v>
+        <v>5.495455974181232</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="B105" t="n">
-        <v>4900000</v>
+        <v>4403000</v>
       </c>
       <c r="C105" t="n">
-        <v>4669901</v>
+        <v>4207844.5</v>
       </c>
       <c r="D105" t="n">
-        <v>4.695897959183673</v>
+        <v>4.432330229389053</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B106" t="n">
-        <v>4900000</v>
+        <v>4200000</v>
       </c>
       <c r="C106" t="n">
-        <v>4670348</v>
+        <v>4018511.5</v>
       </c>
       <c r="D106" t="n">
-        <v>4.686775510204082</v>
+        <v>4.321154761904762</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B107" t="n">
-        <v>2940000</v>
+        <v>5040000</v>
       </c>
       <c r="C107" t="n">
-        <v>3076083.75</v>
+        <v>4825860</v>
       </c>
       <c r="D107" t="n">
-        <v>4.628698979591837</v>
+        <v>4.248809523809524</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="B108" t="n">
-        <v>3640000</v>
+        <v>3290000</v>
       </c>
       <c r="C108" t="n">
-        <v>3483223.5</v>
+        <v>3151444</v>
       </c>
       <c r="D108" t="n">
-        <v>4.307046703296716</v>
+        <v>4.211428571428572</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B109" t="n">
-        <v>3290000</v>
+        <v>4473000</v>
       </c>
       <c r="C109" t="n">
-        <v>3149025.75</v>
+        <v>4639571.5</v>
       </c>
       <c r="D109" t="n">
-        <v>4.284931610942249</v>
+        <v>3.723932483791639</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="B110" t="n">
-        <v>3360000</v>
+        <v>4200000</v>
       </c>
       <c r="C110" t="n">
-        <v>3219712.5</v>
+        <v>4048922</v>
       </c>
       <c r="D110" t="n">
-        <v>4.175223214285714</v>
+        <v>3.597095238095238</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="B111" t="n">
-        <v>3115000</v>
+        <v>4200000</v>
       </c>
       <c r="C111" t="n">
-        <v>2985957.5</v>
+        <v>4056660.75</v>
       </c>
       <c r="D111" t="n">
-        <v>4.142616372391653</v>
+        <v>3.412839285714286</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B112" t="n">
-        <v>6510000</v>
+        <v>4270000</v>
       </c>
       <c r="C112" t="n">
-        <v>6778699</v>
+        <v>4125080.75</v>
       </c>
       <c r="D112" t="n">
-        <v>4.127480798771122</v>
+        <v>3.393893442622951</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B113" t="n">
-        <v>8080940.000000001</v>
+        <v>3990000</v>
       </c>
       <c r="C113" t="n">
-        <v>7754173</v>
+        <v>3865254.5</v>
       </c>
       <c r="D113" t="n">
-        <v>4.043675611995646</v>
+        <v>3.126453634085213</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="B114" t="n">
-        <v>6293000</v>
+        <v>6650000</v>
       </c>
       <c r="C114" t="n">
-        <v>6537681.5</v>
+        <v>6854505</v>
       </c>
       <c r="D114" t="n">
-        <v>3.888153503893214</v>
+        <v>3.075263157894737</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="B115" t="n">
-        <v>3255000</v>
+        <v>6790000</v>
       </c>
       <c r="C115" t="n">
-        <v>3129251.75</v>
+        <v>6987984</v>
       </c>
       <c r="D115" t="n">
-        <v>3.863233486943164</v>
+        <v>2.915817378497791</v>
       </c>
     </row>
     <row r="116">
@@ -2054,178 +2054,178 @@
         <v>4340000</v>
       </c>
       <c r="C116" t="n">
-        <v>4174488.5</v>
+        <v>4227455.5</v>
       </c>
       <c r="D116" t="n">
-        <v>3.813629032258064</v>
+        <v>2.593191244239631</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="B117" t="n">
-        <v>4200000</v>
+        <v>3640000</v>
       </c>
       <c r="C117" t="n">
-        <v>4041252.75</v>
+        <v>3551727.75</v>
       </c>
       <c r="D117" t="n">
-        <v>3.779696428571429</v>
+        <v>2.425061813186826</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B118" t="n">
-        <v>5950000</v>
+        <v>2660000</v>
       </c>
       <c r="C118" t="n">
-        <v>5727611</v>
+        <v>2721599.25</v>
       </c>
       <c r="D118" t="n">
-        <v>3.73763025210084</v>
+        <v>2.315761278195489</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B119" t="n">
-        <v>5950000</v>
+        <v>3220000</v>
       </c>
       <c r="C119" t="n">
-        <v>5736297.5</v>
+        <v>3291428.75</v>
       </c>
       <c r="D119" t="n">
-        <v>3.591638655462185</v>
+        <v>2.218284161490683</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B120" t="n">
-        <v>3010000</v>
+        <v>3360000</v>
       </c>
       <c r="C120" t="n">
-        <v>3115930.25</v>
+        <v>3287667.5</v>
       </c>
       <c r="D120" t="n">
-        <v>3.519277408637874</v>
+        <v>2.152752976190476</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B121" t="n">
-        <v>4403000</v>
+        <v>2940000</v>
       </c>
       <c r="C121" t="n">
-        <v>4253098.5</v>
+        <v>2995410.75</v>
       </c>
       <c r="D121" t="n">
-        <v>3.404531001589825</v>
+        <v>1.884719387755102</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="B122" t="n">
-        <v>6790000</v>
+        <v>3703000</v>
       </c>
       <c r="C122" t="n">
-        <v>7014686.5</v>
+        <v>3765264</v>
       </c>
       <c r="D122" t="n">
-        <v>3.309079528718704</v>
+        <v>1.681447475020267</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B123" t="n">
-        <v>3990000</v>
+        <v>4200000</v>
       </c>
       <c r="C123" t="n">
-        <v>3860629</v>
+        <v>4133008</v>
       </c>
       <c r="D123" t="n">
-        <v>3.242380952380952</v>
+        <v>1.595047619047619</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="B124" t="n">
-        <v>3220000</v>
+        <v>4095000</v>
       </c>
       <c r="C124" t="n">
-        <v>3318753.25</v>
+        <v>4035189.25</v>
       </c>
       <c r="D124" t="n">
-        <v>3.066871118012422</v>
+        <v>1.460579975579976</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B125" t="n">
-        <v>3500000</v>
+        <v>6930000</v>
       </c>
       <c r="C125" t="n">
-        <v>3579837.75</v>
+        <v>6839538.5</v>
       </c>
       <c r="D125" t="n">
-        <v>2.281078571428572</v>
+        <v>1.30536075036075</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B126" t="n">
-        <v>4200000</v>
+        <v>3255000</v>
       </c>
       <c r="C126" t="n">
-        <v>4294570.5</v>
+        <v>3213114.25</v>
       </c>
       <c r="D126" t="n">
-        <v>2.251678571428572</v>
+        <v>1.286812596006145</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B127" t="n">
-        <v>4270000</v>
+        <v>2940000</v>
       </c>
       <c r="C127" t="n">
-        <v>4182066.25</v>
+        <v>2977129</v>
       </c>
       <c r="D127" t="n">
-        <v>2.059338407494145</v>
+        <v>1.262891156462585</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="B128" t="n">
-        <v>7419999.999999999</v>
+        <v>6300000</v>
       </c>
       <c r="C128" t="n">
-        <v>7280382</v>
+        <v>6220770.5</v>
       </c>
       <c r="D128" t="n">
-        <v>1.88164420485174</v>
+        <v>1.257611111111111</v>
       </c>
     </row>
     <row r="129">
@@ -2236,66 +2236,66 @@
         <v>3360000</v>
       </c>
       <c r="C129" t="n">
-        <v>3323065.5</v>
+        <v>3322730.75</v>
       </c>
       <c r="D129" t="n">
-        <v>1.099241071428571</v>
+        <v>1.109203869047619</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B130" t="n">
-        <v>6650000</v>
+        <v>5873000</v>
       </c>
       <c r="C130" t="n">
-        <v>6722883.5</v>
+        <v>5930436</v>
       </c>
       <c r="D130" t="n">
-        <v>1.095992481203008</v>
+        <v>0.9779669674782905</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="B131" t="n">
-        <v>4200000</v>
+        <v>4900000</v>
       </c>
       <c r="C131" t="n">
-        <v>4161787.5</v>
+        <v>4936517.5</v>
       </c>
       <c r="D131" t="n">
-        <v>0.9098214285714286</v>
+        <v>0.7452551020408162</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="B132" t="n">
-        <v>5873000</v>
+        <v>3353000</v>
       </c>
       <c r="C132" t="n">
-        <v>5843838</v>
+        <v>3361860.75</v>
       </c>
       <c r="D132" t="n">
-        <v>0.4965435041716329</v>
+        <v>0.2642633462570832</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="B133" t="n">
-        <v>4473000</v>
+        <v>4340000</v>
       </c>
       <c r="C133" t="n">
-        <v>4471301.5</v>
+        <v>4329968.5</v>
       </c>
       <c r="D133" t="n">
-        <v>0.03797227811312318</v>
+        <v>0.2311405529953917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>